<commit_message>
Found correlation of criteria
</commit_message>
<xml_diff>
--- a/Fedrizzi.xlsx
+++ b/Fedrizzi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\zevgg\coding\carleton\math295\VotingSystems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9DD974-0575-4AD7-B75A-6C3D74B4F405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843B6492-696D-4AE7-8BB4-E6874C5530FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{E0D7ADB8-B075-40B2-A50B-73CB8A34BECA}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8964" xr2:uid="{E0D7ADB8-B075-40B2-A50B-73CB8A34BECA}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>Condorcet winner</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>Poly0mial time</t>
-  </si>
-  <si>
-    <t>Instant-ru0ff voting</t>
   </si>
   <si>
     <t># Fulfilled</t>
@@ -584,9 +581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4102CEC-C8B8-4176-B9BC-A2EF591A9FF2}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,10 +593,10 @@
   <sheetData>
     <row r="1" spans="1:18" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -632,7 +629,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>29</v>
@@ -647,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1106,9 +1103,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -1564,7 +1561,7 @@
     </row>
     <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -1678,7 +1675,7 @@
     </row>
     <row r="20" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -1849,7 +1846,7 @@
     </row>
     <row r="23" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -1906,7 +1903,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
@@ -1963,7 +1960,7 @@
     </row>
     <row r="25" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
@@ -2028,7 +2025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D06C60-F13B-456C-8D98-DA597CA67642}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
@@ -2061,7 +2058,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>19</v>
@@ -2085,13 +2082,13 @@
         <v>25</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U1" s="4" t="s">
         <v>27</v>
@@ -2100,13 +2097,13 @@
         <v>28</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
@@ -2919,7 +2916,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" cm="1">
         <f t="array" ref="B10">SUMPRODUCT(--('Raw Data'!$B$2:$Q$2='Raw Data'!$B10:$Q10))/16</f>
@@ -3727,7 +3724,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" cm="1">
         <f t="array" ref="B18">SUMPRODUCT(--('Raw Data'!$B$2:$Q$2='Raw Data'!$B18:$Q18))/16</f>
@@ -3929,7 +3926,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" cm="1">
         <f t="array" ref="B20">SUMPRODUCT(--('Raw Data'!$B$2:$Q$2='Raw Data'!$B20:$Q20))/16</f>
@@ -4232,7 +4229,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" cm="1">
         <f t="array" ref="B23">SUMPRODUCT(--('Raw Data'!$B$2:$Q$2='Raw Data'!$B23:$Q23))/16</f>
@@ -4333,7 +4330,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" cm="1">
         <f t="array" ref="B24">SUMPRODUCT(--('Raw Data'!$B$2:$Q$2='Raw Data'!$B24:$Q24))/16</f>
@@ -4434,7 +4431,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" cm="1">
         <f t="array" ref="B25">SUMPRODUCT(--('Raw Data'!$B$2:$Q$2='Raw Data'!$B25:$Q25))/16</f>

</xml_diff>